<commit_message>
Am modificat fisierul de recapitulare la bazele marketingului
</commit_message>
<xml_diff>
--- a/Bazele_Marketingului/Recapitulare_17_04_2022.xlsx
+++ b/Bazele_Marketingului/Recapitulare_17_04_2022.xlsx
@@ -482,7 +482,7 @@
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="35">
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="1" fillId="2" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -557,17 +557,10 @@
     </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf fontId="0" fillId="0" borderId="0" numFmtId="9" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
     <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf fontId="2" fillId="0" borderId="0" numFmtId="2" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1196,7 +1189,7 @@
         <v>6000</v>
       </c>
       <c r="G7" s="7">
-        <f>SUM(B7:F7)</f>
+        <f t="shared" ref="G7:G9" si="0">SUM(B7:F7)</f>
         <v>20000</v>
       </c>
       <c r="H7" s="12">
@@ -1231,7 +1224,7 @@
         <v>7000</v>
       </c>
       <c r="G8" s="7">
-        <f>SUM(B8:F8)</f>
+        <f t="shared" si="0"/>
         <v>13000</v>
       </c>
       <c r="H8" s="12">
@@ -1269,7 +1262,7 @@
         <v>2000</v>
       </c>
       <c r="G9" s="7">
-        <f>SUM(B9:F9)</f>
+        <f t="shared" si="0"/>
         <v>14000</v>
       </c>
       <c r="H9" s="12">
@@ -1583,17 +1576,17 @@
       <c r="G28" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="H28" s="32"/>
+      <c r="H28" s="28"/>
       <c r="I28" s="28" t="s">
         <v>55</v>
       </c>
-      <c r="J28" s="33">
+      <c r="J28" s="32">
         <v>1</v>
       </c>
       <c r="K28" s="30" t="s">
         <v>56</v>
       </c>
-      <c r="L28" s="34"/>
+      <c r="L28" s="30"/>
     </row>
     <row r="29" ht="14.25">
       <c r="A29" s="7" t="s">
@@ -1615,10 +1608,10 @@
         <v>6000</v>
       </c>
       <c r="G29" s="7">
-        <f>SUM(B29:F29)</f>
+        <f t="shared" ref="G29:G32" si="1">SUM(B29:F29)</f>
         <v>20000</v>
       </c>
-      <c r="L29" s="34"/>
+      <c r="L29" s="30"/>
     </row>
     <row r="30" ht="14.25">
       <c r="A30" s="7" t="s">
@@ -1640,18 +1633,18 @@
         <v>7000</v>
       </c>
       <c r="G30" s="7">
-        <f>SUM(B30:F30)</f>
+        <f t="shared" si="1"/>
         <v>13000</v>
       </c>
-      <c r="H30" s="35" t="s">
+      <c r="H30" s="33" t="s">
         <v>57</v>
       </c>
-      <c r="I30" s="34"/>
-      <c r="J30" s="34"/>
-      <c r="K30" s="35" t="s">
+      <c r="I30" s="30"/>
+      <c r="J30" s="30"/>
+      <c r="K30" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="L30" s="34"/>
+      <c r="L30" s="30"/>
     </row>
     <row r="31" ht="14.25">
       <c r="A31" s="7" t="s">
@@ -1673,14 +1666,14 @@
         <v>2000</v>
       </c>
       <c r="G31" s="7">
-        <f>SUM(B31:F31)</f>
+        <f t="shared" si="1"/>
         <v>14000</v>
       </c>
-      <c r="H31" s="34"/>
-      <c r="I31" s="34"/>
-      <c r="J31" s="34"/>
-      <c r="K31" s="34"/>
-      <c r="L31" s="34"/>
+      <c r="H31" s="30"/>
+      <c r="I31" s="30"/>
+      <c r="J31" s="30"/>
+      <c r="K31" s="30"/>
+      <c r="L31" s="30"/>
     </row>
     <row r="32" ht="14.25">
       <c r="A32" s="7" t="s">
@@ -1702,14 +1695,14 @@
         <v>5000</v>
       </c>
       <c r="G32" s="7">
-        <f>SUM(B32:F32)</f>
+        <f t="shared" si="1"/>
         <v>7000</v>
       </c>
-      <c r="H32" s="34"/>
-      <c r="I32" s="34"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="34"/>
-      <c r="L32" s="34"/>
+      <c r="H32" s="30"/>
+      <c r="I32" s="30"/>
+      <c r="J32" s="30"/>
+      <c r="K32" s="30"/>
+      <c r="L32" s="30"/>
     </row>
     <row r="33" ht="71.25">
       <c r="A33" s="7" t="s">
@@ -1739,17 +1732,17 @@
         <f>SUM(G29:G32)</f>
         <v>54000</v>
       </c>
-      <c r="H33" s="35" t="s">
+      <c r="H33" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="I33" s="36" t="s">
+      <c r="I33" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="J33" s="34"/>
-      <c r="K33" s="35" t="s">
+      <c r="J33" s="30"/>
+      <c r="K33" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="L33" s="34"/>
+      <c r="L33" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="9">
@@ -1765,7 +1758,7 @@
   </mergeCells>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
@@ -1848,14 +1841,14 @@
         <v>0</v>
       </c>
       <c r="G2" s="22">
-        <f>SUM(B2:F2)</f>
+        <f t="shared" ref="G2:G5" si="2">SUM(B2:F2)</f>
         <v>14300</v>
       </c>
-      <c r="H2" s="37">
+      <c r="H2" s="34">
         <f>G2/G6*100</f>
         <v>16.342857142857142</v>
       </c>
-      <c r="I2" s="37">
+      <c r="I2" s="34">
         <f>G2/G3</f>
         <v>0.35221674876847292</v>
       </c>
@@ -1863,7 +1856,7 @@
         <f>3/5*100</f>
         <v>60</v>
       </c>
-      <c r="K2" s="37">
+      <c r="K2" s="34">
         <f>SUM(B6,C6,D6)/G6*100</f>
         <v>71.657142857142858</v>
       </c>
@@ -1891,21 +1884,21 @@
         <v>8300</v>
       </c>
       <c r="G3" s="22">
-        <f>SUM(B3:F3)</f>
+        <f t="shared" si="2"/>
         <v>40600</v>
       </c>
-      <c r="H3" s="37">
+      <c r="H3" s="34">
         <f>G3/G6*100</f>
         <v>46.400000000000006</v>
       </c>
-      <c r="I3" s="37">
+      <c r="I3" s="34">
         <f>G3/G5</f>
         <v>1.6504065040650406</v>
       </c>
       <c r="J3" s="22">
         <v>100</v>
       </c>
-      <c r="K3" s="37">
+      <c r="K3" s="34">
         <f>SUM(B6:F6)/G6*100</f>
         <v>100</v>
       </c>
@@ -1933,14 +1926,14 @@
         <v>0</v>
       </c>
       <c r="G4" s="22">
-        <f>SUM(B4:F4)</f>
+        <f t="shared" si="2"/>
         <v>8000</v>
       </c>
-      <c r="H4" s="37">
+      <c r="H4" s="34">
         <f>G4/G6*100</f>
         <v>9.1428571428571423</v>
       </c>
-      <c r="I4" s="37">
+      <c r="I4" s="34">
         <f>G4/G3</f>
         <v>0.19704433497536947</v>
       </c>
@@ -1948,9 +1941,9 @@
         <f>3/5*100</f>
         <v>60</v>
       </c>
-      <c r="K4" s="37">
-        <f>SUM(B4,C4,E4)/G6*100</f>
-        <v>9.1428571428571423</v>
+      <c r="K4" s="34">
+        <f>SUM(B6,C6,E6)/G6*100</f>
+        <v>62.742857142857147</v>
       </c>
     </row>
     <row r="5" ht="14.25">
@@ -1973,14 +1966,14 @@
         <v>6300</v>
       </c>
       <c r="G5" s="22">
-        <f>SUM(B5:F5)</f>
+        <f t="shared" si="2"/>
         <v>24600</v>
       </c>
-      <c r="H5" s="37">
+      <c r="H5" s="34">
         <f>G5/G6*100</f>
         <v>28.114285714285714</v>
       </c>
-      <c r="I5" s="37">
+      <c r="I5" s="34">
         <f>G5/G3</f>
         <v>0.60591133004926112</v>
       </c>
@@ -1988,9 +1981,9 @@
         <f>4/5*100</f>
         <v>80</v>
       </c>
-      <c r="K5" s="37">
-        <f>SUM(B5,C5,D5,F5)/G6*100</f>
-        <v>28.114285714285714</v>
+      <c r="K5" s="34">
+        <f>SUM(B6,C6,D6,F6)/G6*100</f>
+        <v>88.342857142857142</v>
       </c>
     </row>
     <row r="6" ht="14.25">
@@ -2027,7 +2020,9 @@
       </c>
       <c r="I6" s="22"/>
       <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
+      <c r="K6" s="22" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="11" ht="14.25">
       <c r="B11" t="s">
@@ -2054,7 +2049,7 @@
         <v>14300</v>
       </c>
       <c r="E12">
-        <f>(D12-C12)/C12*100</f>
+        <f t="shared" ref="E12:E15" si="3">(D12-C12)/C12*100</f>
         <v>-28.499999999999996</v>
       </c>
       <c r="F12" t="s">
@@ -2072,7 +2067,7 @@
         <v>40600</v>
       </c>
       <c r="E13">
-        <f>(D13-C13)/C13*100</f>
+        <f t="shared" si="3"/>
         <v>100.99009900990099</v>
       </c>
       <c r="F13" t="s">
@@ -2090,7 +2085,7 @@
         <v>8000</v>
       </c>
       <c r="E14">
-        <f>(D14-C14)/C14*100</f>
+        <f t="shared" si="3"/>
         <v>105.12820512820514</v>
       </c>
       <c r="F14" t="s">
@@ -2108,7 +2103,7 @@
         <v>24600</v>
       </c>
       <c r="E15">
-        <f>(D15-C15)/C15*100</f>
+        <f t="shared" si="3"/>
         <v>59.740259740259738</v>
       </c>
       <c r="F15" t="s">
@@ -2118,7 +2113,7 @@
   </sheetData>
   <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.70078740157480324" right="0.70078740157480324" top="0.75196850393700787" bottom="0.75196850393700787" header="0.29999999999999999" footer="0.29999999999999999"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="4294967295" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="2147483648" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="600" verticalDpi="600" copies="1"/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>